<commit_message>
3rd version half done
</commit_message>
<xml_diff>
--- a/revised/peshawar/peshawar.xlsx
+++ b/revised/peshawar/peshawar.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D619BF-C44E-46BB-BCB0-86EC21933568}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEC9E00-3513-4722-8A7A-0E715FBDD4B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annual distribution" sheetId="2" r:id="rId1"/>
@@ -80,12 +80,6 @@
     <t>Autam</t>
   </si>
   <si>
-    <t>Passenager</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>No Damge to PR</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>No of Injuries</t>
+  </si>
+  <si>
+    <t>Passenager train</t>
+  </si>
+  <si>
+    <t>Goods Train</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -839,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28029C6-2094-4F19-B9E2-17CE7D370274}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -942,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC59E211-7C54-4EF4-90AF-28915C91AD3D}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
@@ -956,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5">
@@ -1056,7 +1056,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1069,13 +1069,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.5">
@@ -1190,7 +1190,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1203,16 +1203,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.5">

</xml_diff>

<commit_message>
changes in peshawar analysis
</commit_message>
<xml_diff>
--- a/revised/peshawar/peshawar.xlsx
+++ b/revised/peshawar/peshawar.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEC9E00-3513-4722-8A7A-0E715FBDD4B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6616BD2A-2BC6-4A5E-8DC5-5035D97108E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="annual distribution" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -150,7 +150,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -173,6 +173,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -184,7 +195,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -235,6 +246,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -727,7 +741,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -837,15 +851,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28029C6-2094-4F19-B9E2-17CE7D370274}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
+    <row r="1" spans="1:4" ht="45">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -855,8 +869,11 @@
       <c r="C1" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="31">
+      <c r="D1" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31">
       <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
@@ -866,8 +883,11 @@
       <c r="C2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="31">
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="31">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -875,6 +895,9 @@
         <v>0</v>
       </c>
       <c r="C3" s="8">
+        <v>17</v>
+      </c>
+      <c r="D3">
         <v>17</v>
       </c>
     </row>
@@ -942,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC59E211-7C54-4EF4-90AF-28915C91AD3D}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>